<commit_message>
rectification de la deuxième slice
</commit_message>
<xml_diff>
--- a/Cspecs.xlsx
+++ b/Cspecs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laubr\Desktop\Poker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laubr\Desktop\Poker2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{488BEFBC-B81F-4458-B56F-AF3AB83133C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CF62F0F3-2B35-44CC-930C-73F98C8DBFDA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{17C324D7-EC0A-4407-B813-DAAD437C8DEF}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t>Le logiciel reconnait deux mains de une carte entrées par l'utilisateur et les compare par leur hauteur. Le logiciel ne gère qu'un paquet contenant que la famille pique.</t>
   </si>
   <si>
-    <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte de la combinaison: couleur. Le logiciel ne gère qu'un paquet contenant que la famille pique.</t>
-  </si>
-  <si>
     <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte des combinaisons: brelan, suite, couleur, full, carré et quinte flush.</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>Le logiciel est capable de reconnaitre une main malgré le nombre d'espace mis par l'utilisateur entre chaque carte, de plus la famille d'une carte peut être spécifiée par majuscule ou miniscule.</t>
+  </si>
+  <si>
+    <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte de la combinaison: couleur. Le logiciel ne gère qu'un paquet contenant que la famille pique, le logiciel gère les erreurs de saisie.</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +627,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -650,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -687,16 +687,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -719,7 +719,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -742,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -765,7 +765,7 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9">
         <v>5</v>
@@ -788,7 +788,7 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -828,13 +828,13 @@
         <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -848,16 +848,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D13" t="s">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13">
         <v>7</v>

</xml_diff>

<commit_message>
rectification de la slice 12
</commit_message>
<xml_diff>
--- a/Cspecs.xlsx
+++ b/Cspecs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laubr\Desktop\Poker2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CF62F0F3-2B35-44CC-930C-73F98C8DBFDA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AFCEBA01-0E03-4BDD-96D8-F95CC761B06A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{17C324D7-EC0A-4407-B813-DAAD437C8DEF}"/>
   </bookViews>
@@ -183,10 +183,10 @@
     <t>Le logiciel est moins plus flexible pour l'écriture des mains.</t>
   </si>
   <si>
-    <t>Le logiciel est capable de reconnaitre une main malgré le nombre d'espace mis par l'utilisateur entre chaque carte, de plus la famille d'une carte peut être spécifiée par majuscule ou miniscule.</t>
-  </si>
-  <si>
     <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte de la combinaison: couleur. Le logiciel ne gère qu'un paquet contenant que la famille pique, le logiciel gère les erreurs de saisie.</t>
+  </si>
+  <si>
+    <t>Le logiciel est capable de reconnaitre une main malgré le nombre d'espace mis par l'utilisateur entre chaque carte, de plus la famille d'une carte peut être spécifiée par majuscule ou miniscule. La saisie de carte est plus simple, les têtes peuvent être tapées avec leur initiale.</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +627,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -857,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F13">
         <v>7</v>

</xml_diff>

<commit_message>
rectification de la 12ème slice
</commit_message>
<xml_diff>
--- a/Cspecs.xlsx
+++ b/Cspecs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laubr\Desktop\Poker2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AFCEBA01-0E03-4BDD-96D8-F95CC761B06A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CE9D023E-D28B-4A68-887D-6E16E995F145}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{17C324D7-EC0A-4407-B813-DAAD437C8DEF}"/>
   </bookViews>
@@ -183,10 +183,10 @@
     <t>Le logiciel est moins plus flexible pour l'écriture des mains.</t>
   </si>
   <si>
-    <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte de la combinaison: couleur. Le logiciel ne gère qu'un paquet contenant que la famille pique, le logiciel gère les erreurs de saisie.</t>
-  </si>
-  <si>
-    <t>Le logiciel est capable de reconnaitre une main malgré le nombre d'espace mis par l'utilisateur entre chaque carte, de plus la famille d'une carte peut être spécifiée par majuscule ou miniscule. La saisie de carte est plus simple, les têtes peuvent être tapées avec leur initiale.</t>
+    <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte des combinaisons: couleur et suite. Le logiciel ne gère qu'un paquet contenant que la famille pique, le logiciel gère les erreurs de saisie et affiche le résultat comme les spécifications.  La saisie de carte est plus simple, les têtes peuvent être tapées avec leur initiale.</t>
+  </si>
+  <si>
+    <t>La famille d'une carte peut être spécifiée par majuscule ou miniscule. La saisie de carte est plus simple, les têtes peuvent être tapées avec leur initiale.</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changements mineurs sur les phrases affichées
</commit_message>
<xml_diff>
--- a/Cspecs.xlsx
+++ b/Cspecs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laubr\Desktop\Poker2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laubr\Desktop\Projets\Poker2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{66E6950B-EA5A-488E-A714-C6A2303E0222}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E4A834B-3024-447C-974D-30936DFDC2AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{17C324D7-EC0A-4407-B813-DAAD437C8DEF}"/>
   </bookViews>
@@ -183,10 +183,10 @@
     <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte des combinaisons: couleur et suite. Le logiciel ne gère qu'un paquet contenant que la famille pique, le logiciel gère les erreurs de saisie et affiche le résultat comme les spécifications.  La saisie de carte est plus simple, les têtes peuvent être tapées avec leur initiale.</t>
   </si>
   <si>
-    <t>La famille d'une carte peut être spécifiée par majuscule ou miniscule. La saisie de carte est plus simple, les têtes peuvent être tapées avec leur initiale.</t>
-  </si>
-  <si>
     <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte de la combinaison: double paires, quinte et couleur. Le logiciel ne gère qu'un paquet contenant les familles pique et cœur. Le logiciel gère les égalités.</t>
+  </si>
+  <si>
+    <t>La famille d'une carte peut être spécifiée par majuscule ou miniscule. Les espaces en trop entre chaque cartes sont ignorés.</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -857,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F13">
         <v>7</v>

</xml_diff>

<commit_message>
changement du xls au niveau des slices
</commit_message>
<xml_diff>
--- a/Cspecs.xlsx
+++ b/Cspecs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laubr\Desktop\Projets\Poker2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E4A834B-3024-447C-974D-30936DFDC2AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F3507B2-35F4-43F5-B080-E4ECC299CBCE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{17C324D7-EC0A-4407-B813-DAAD437C8DEF}"/>
   </bookViews>
@@ -544,7 +544,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +739,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
changement des notes de difficultés sur le xls
</commit_message>
<xml_diff>
--- a/Cspecs.xlsx
+++ b/Cspecs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laubr\Desktop\Projets\Poker2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F3507B2-35F4-43F5-B080-E4ECC299CBCE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7C919120-C6ED-4594-9312-99DCF974BEDB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{17C324D7-EC0A-4407-B813-DAAD437C8DEF}"/>
   </bookViews>
@@ -544,7 +544,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +748,7 @@
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -771,7 +771,7 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changement mineurs sur le xls
</commit_message>
<xml_diff>
--- a/Cspecs.xlsx
+++ b/Cspecs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laubr\Desktop\Projets\Poker2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laubr\Desktop\Lucas Aubron\Projets\Poker2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CE62BF6A-4EC3-42F3-BFD8-067CCD5443FB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AECA9328-D6A8-4C69-B24B-E7CE1535E4CD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{17C324D7-EC0A-4407-B813-DAAD437C8DEF}"/>
   </bookViews>
@@ -177,12 +177,6 @@
     <t>Stabilité lors de l'entrée des mains</t>
   </si>
   <si>
-    <t>Le logiciel est moins plus flexible pour l'écriture des mains.</t>
-  </si>
-  <si>
-    <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte des combinaisons: couleur et suite. Le logiciel ne gère qu'un paquet contenant que la famille pique, le logiciel gère les erreurs de saisie et affiche le résultat comme les spécifications.  La saisie de carte est plus simple, les têtes peuvent être tapées avec leur initiale.</t>
-  </si>
-  <si>
     <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte de la combinaison: double paires, quinte et couleur. Le logiciel ne gère qu'un paquet contenant les familles pique et cœur. Le logiciel gère les égalités.</t>
   </si>
   <si>
@@ -196,6 +190,12 @@
   </si>
   <si>
     <t>Le logiciel est complet, il reconnaît les erreurs suivantes: mauvaise saisie d'une famille d'une carte, mauvaise saisie d'une valeur d'une carte, saisie de deux cartes identiques dans le jeu, saisie d'une main de taille indaptée (ie !=5).</t>
+  </si>
+  <si>
+    <t>Le logiciel est plus flexible pour l'écriture des mains.</t>
+  </si>
+  <si>
+    <t>Le logiciel reconnait deux mains de cinq cartes entrées par l'utilisateur et indique laquelle est la plus forte sans tenir compte des combinaisons: couleur et suite. Le logiciel ne gère qu'un paquet contenant que la famille pique, le logiciel gère le cas où une même carte est utilisée deux fois, et affiche le résultat comme les spécifications.  La saisie de carte est plus simple, les têtes peuvent être tapées avec leur initiale.</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -659,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -860,13 +860,13 @@
         <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13">
         <v>7</v>
@@ -880,16 +880,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F14">
         <v>7</v>

</xml_diff>